<commit_message>
added quadruple zeta for cl- in ice
</commit_message>
<xml_diff>
--- a/cl_0_1_6_water_added_in_ice_saop.xlsx
+++ b/cl_0_1_6_water_added_in_ice_saop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/Thesis_graphs_binder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/opoku/Desktop/HCl_project_graphs_binder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98981FBE-86A8-8749-8305-8D27A500D18E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2352750D-9D01-5548-BFFC-1A42733EA348}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="480" windowWidth="25060" windowHeight="14920" xr2:uid="{C1ADF71C-6822-4348-A305-5C9E8C2279D3}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="21120" windowHeight="14920" xr2:uid="{C1ADF71C-6822-4348-A305-5C9E8C2279D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A4:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>